<commit_message>
Added config reader file updated the project structure Working on one more sub-project inside this project
</commit_message>
<xml_diff>
--- a/resources/data3.xlsx
+++ b/resources/data3.xlsx
@@ -1,92 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bughr\PycharmProjects\SeleniumPython\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8717559-4127-492C-A1A9-ADC62ECCE47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5760" yWindow="1368" windowWidth="17280" windowHeight="8976" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>userId</t>
-  </si>
-  <si>
-    <t>test1@me.com</t>
-  </si>
-  <si>
-    <t>admin@123</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>test2@me.com</t>
-  </si>
-  <si>
-    <t>admin@223</t>
-  </si>
-  <si>
-    <t>user3</t>
-  </si>
-  <si>
-    <t>test3@me.com</t>
-  </si>
-  <si>
-    <t>admin@323</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -103,31 +53,90 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -393,74 +402,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col width="6" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.6640625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="10.77734375" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="8.88671875" customWidth="1" style="1" min="4" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>userId</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>password</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>user1</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>test1@me.com</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>admin@123</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>user2</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>test2@me.com</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>admin@223</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>user3</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>test3@me.com</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>admin@323</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{782D4493-9783-4777-B1A7-233F74B164E7}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{21CA6CE5-FC52-444B-9465-F28EEC2722B0}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{5C7FD918-4F61-4B20-9B64-51778486F0B7}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{BEB78F3C-62A5-4636-AED5-95F82A8DA2AE}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{160521D8-6FBC-4CD8-BEA8-738FDE8BF2DE}"/>
-    <hyperlink ref="C4" r:id="rId6" xr:uid="{FA50B23E-4786-49EF-B716-3700451EDA92}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>